<commit_message>
updated timeline xls and eventos.txt
</commit_message>
<xml_diff>
--- a/docs/eventos_timeline.xlsx
+++ b/docs/eventos_timeline.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
   <si>
     <t>Sistema</t>
   </si>
@@ -74,6 +74,120 @@
   </si>
   <si>
     <t>Interfaces con la AFIP, Banco Nación y Cámaras Judiciales.</t>
+  </si>
+  <si>
+    <t>Plan Nacional de Regularización del Trabajo (PNRT)</t>
+  </si>
+  <si>
+    <t>Secretaría de Trabajo</t>
+  </si>
+  <si>
+    <t>Inspector Digital (INDI)</t>
+  </si>
+  <si>
+    <t>Sistema Ley 18695 (CPL)</t>
+  </si>
+  <si>
+    <t>Inspector Digital Competencia Federal (INDICFED)</t>
+  </si>
+  <si>
+    <t>Registro Único de Inspecciones, Infracciones y Sanciones (RUIIS) </t>
+  </si>
+  <si>
+    <t>Sistema de registro de Empresas de Servicios Eventuales</t>
+  </si>
+  <si>
+    <t>Sistema de Gestión de Ordenes de Inspección (GOI)</t>
+  </si>
+  <si>
+    <t>Sistema de Inspección de Trabajo Infantil Prohibido y Trabajo Adolescente Irregular (COODITIA)</t>
+  </si>
+  <si>
+    <t>Biblioteca digital de Convenios Colectivos de Trabajo</t>
+  </si>
+  <si>
+    <t>Sistema de Gestión de la Negociación Colectiva (DRT)</t>
+  </si>
+  <si>
+    <t>Sistema de Negociación Colectiva (actualmente en desarrollo)</t>
+  </si>
+  <si>
+    <t>DNAS</t>
+  </si>
+  <si>
+    <t>Sistema de Gestión del Programa de Recuperación Productiva (RePro)</t>
+  </si>
+  <si>
+    <t>Sistema Público de Registro de Empresas y Nómina de Trabajadores al Programa de Recuperación Productiva (Empresas en RePro)</t>
+  </si>
+  <si>
+    <t>Sistema del SECLO</t>
+  </si>
+  <si>
+    <t>Diarios y Revistas</t>
+  </si>
+  <si>
+    <t>Asistir</t>
+  </si>
+  <si>
+    <t>Sistema del Tribunal de Trabajo Doméstico</t>
+  </si>
+  <si>
+    <t>Sistema de Encuestas de la Red de Empresas contra el Trabajo Infantil (RedECTI)</t>
+  </si>
+  <si>
+    <t>Portal de empleo</t>
+  </si>
+  <si>
+    <t>Secretaría de Empleo</t>
+  </si>
+  <si>
+    <t>Sistema de Gestión de Proyectos</t>
+  </si>
+  <si>
+    <t>Sistema de Fiscalización y seguimiento de proyectos</t>
+  </si>
+  <si>
+    <t>Sistema de Liquidación de planes sociales</t>
+  </si>
+  <si>
+    <t>Sistema de Administración de Tarjetas Magnéticas</t>
+  </si>
+  <si>
+    <t>Sistema de Mesa de Entradas General</t>
+  </si>
+  <si>
+    <t>Sistema de Resoluciones y Normativa</t>
+  </si>
+  <si>
+    <t>Servicio de Firma digital de Normativa</t>
+  </si>
+  <si>
+    <t>Sistema de Oficios Judiciales</t>
+  </si>
+  <si>
+    <t>Sistema de Notificaciones</t>
+  </si>
+  <si>
+    <t>Sistema de Sumarios Administrativos</t>
+  </si>
+  <si>
+    <t>Sistema de Liquidación de Viáticos</t>
+  </si>
+  <si>
+    <t>Sistema de Liquidación de Fondos Rotatorios</t>
+  </si>
+  <si>
+    <t>Sistema de Concursos (en uso en múltiples organismos SINEP)</t>
+  </si>
+  <si>
+    <t>Sistema de Postulantes</t>
+  </si>
+  <si>
+    <t>Sistema del Centro de Asesoramiento Laboral (Callcenter)</t>
+  </si>
+  <si>
+    <t>Sistema de Dictámenes</t>
   </si>
 </sst>
 </file>
@@ -208,6 +322,302 @@
         <v>20</v>
       </c>
     </row>
+    <row r="5">
+      <c t="s" r="A5">
+        <v>21</v>
+      </c>
+      <c t="s" r="D5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" r="A6">
+        <v>23</v>
+      </c>
+      <c t="s" r="D6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7">
+      <c t="s" r="A7">
+        <v>24</v>
+      </c>
+      <c t="s" r="D7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8">
+      <c t="s" r="A8">
+        <v>25</v>
+      </c>
+      <c t="s" r="D8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9">
+      <c t="s" r="A9">
+        <v>26</v>
+      </c>
+      <c t="s" r="D9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10">
+      <c t="s" r="A10">
+        <v>27</v>
+      </c>
+      <c t="s" r="D10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11">
+      <c t="s" r="A11">
+        <v>28</v>
+      </c>
+      <c t="s" r="D11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" r="A12">
+        <v>29</v>
+      </c>
+      <c t="s" r="D12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" r="A13">
+        <v>30</v>
+      </c>
+      <c t="s" r="D13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14">
+      <c t="s" r="A14">
+        <v>31</v>
+      </c>
+      <c t="s" r="D14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15">
+      <c t="s" r="A15">
+        <v>32</v>
+      </c>
+      <c t="s" r="D15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16">
+      <c t="s" r="A16">
+        <v>33</v>
+      </c>
+      <c t="s" r="D16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17">
+      <c t="s" r="A17">
+        <v>34</v>
+      </c>
+      <c t="s" r="D17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18">
+      <c t="s" r="A18">
+        <v>35</v>
+      </c>
+      <c t="s" r="D18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" r="A19">
+        <v>36</v>
+      </c>
+      <c t="s" r="D19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20">
+      <c t="s" r="A20">
+        <v>37</v>
+      </c>
+      <c t="s" r="D20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" r="A21">
+        <v>38</v>
+      </c>
+      <c t="s" r="D21">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22">
+      <c t="s" r="A22">
+        <v>39</v>
+      </c>
+      <c t="s" r="D22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23">
+      <c t="s" r="A23">
+        <v>40</v>
+      </c>
+      <c t="s" r="D23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c t="s" r="A24">
+        <v>41</v>
+      </c>
+      <c t="s" r="D24">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25">
+      <c t="s" r="A25">
+        <v>43</v>
+      </c>
+      <c t="s" r="D25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26">
+      <c t="s" r="A26">
+        <v>44</v>
+      </c>
+      <c t="s" r="D26">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27">
+      <c t="s" r="A27">
+        <v>45</v>
+      </c>
+      <c t="s" r="D27">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28">
+      <c t="s" r="A28">
+        <v>46</v>
+      </c>
+      <c t="s" r="D28">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29">
+      <c t="s" r="A29">
+        <v>47</v>
+      </c>
+      <c t="s" r="D29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30">
+      <c t="s" r="A30">
+        <v>48</v>
+      </c>
+      <c t="s" r="D30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31">
+      <c t="s" r="A31">
+        <v>49</v>
+      </c>
+      <c t="s" r="D31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32">
+      <c t="s" r="A32">
+        <v>50</v>
+      </c>
+      <c t="s" r="D32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33">
+      <c t="s" r="A33">
+        <v>51</v>
+      </c>
+      <c t="s" r="D33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34">
+      <c t="s" r="A34">
+        <v>12</v>
+      </c>
+      <c t="s" r="D34">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35">
+      <c t="s" r="A35">
+        <v>52</v>
+      </c>
+      <c t="s" r="D35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36">
+      <c t="s" r="A36">
+        <v>53</v>
+      </c>
+      <c t="s" r="D36">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37">
+      <c t="s" r="A37">
+        <v>54</v>
+      </c>
+      <c t="s" r="D37">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38">
+      <c t="s" r="A38">
+        <v>55</v>
+      </c>
+      <c t="s" r="D38">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39">
+      <c t="s" r="A39">
+        <v>56</v>
+      </c>
+      <c t="s" r="D39">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40">
+      <c t="s" r="A40">
+        <v>57</v>
+      </c>
+      <c t="s" r="D40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41">
+      <c t="s" r="A41">
+        <v>58</v>
+      </c>
+      <c t="s" r="D41">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new events, adjusted styles
</commit_message>
<xml_diff>
--- a/docs/eventos_timeline.xlsx
+++ b/docs/eventos_timeline.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="123">
   <si>
     <t>status</t>
   </si>
@@ -68,6 +68,9 @@
     <t>http://juicios/</t>
   </si>
   <si>
+    <t>ok</t>
+  </si>
+  <si>
     <t>2006-01</t>
   </si>
   <si>
@@ -221,9 +224,6 @@
     <t>Sistema de Mesa de Entradas General</t>
   </si>
   <si>
-    <t>ok</t>
-  </si>
-  <si>
     <t>1999-10</t>
   </si>
   <si>
@@ -264,6 +264,12 @@
   </si>
   <si>
     <t>Sistema de Sumarios Administrativos</t>
+  </si>
+  <si>
+    <t>falta data</t>
+  </si>
+  <si>
+    <t>falta data!!!</t>
   </si>
   <si>
     <t>2010-06</t>
@@ -519,8 +525,8 @@
   </sheetPr>
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A17" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F25" activeCellId="0" pane="topLeft" sqref="F25"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E1" activeCellId="0" pane="topLeft" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -595,296 +601,304 @@
       <c r="D4" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="E4" s="0" t="s">
+        <v>17</v>
+      </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="5">
       <c r="C5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="6">
       <c r="C6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="7">
       <c r="C7" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="8">
       <c r="C8" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="9">
       <c r="C9" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="11">
       <c r="C11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="12">
       <c r="C12" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="13">
       <c r="C13" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="14">
       <c r="C14" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="15">
       <c r="C15" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="16">
       <c r="C16" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="17">
       <c r="C17" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="18">
       <c r="C18" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="19">
       <c r="C19" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="20">
       <c r="C20" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="22">
       <c r="C22" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="24">
       <c r="C24" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="25">
       <c r="C25" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="26">
       <c r="C26" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="27">
       <c r="C27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>60</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="28">
       <c r="C28" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="29">
       <c r="C29" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="30">
       <c r="C30" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="31">
       <c r="C31" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="F31" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="32">
       <c r="C32" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>69</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="33">
@@ -892,13 +906,13 @@
         <v>70</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>71</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="34">
@@ -906,7 +920,7 @@
         <v>72</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="35">
@@ -914,10 +928,10 @@
         <v>73</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="36">
@@ -928,16 +942,16 @@
         <v>75</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>76</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="37">
@@ -947,11 +961,14 @@
       <c r="C37" s="0" t="s">
         <v>77</v>
       </c>
+      <c r="E37" s="0" t="s">
+        <v>17</v>
+      </c>
       <c r="F37" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H37" s="0" t="s">
         <v>78</v>
@@ -970,182 +987,191 @@
       <c r="C38" s="0" t="s">
         <v>82</v>
       </c>
+      <c r="D38" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>84</v>
+      </c>
       <c r="F38" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="39">
       <c r="C39" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L39" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="40">
       <c r="C40" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K40" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L40" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="41">
       <c r="C41" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="42">
       <c r="C42" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D42" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H42" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="43">
       <c r="C43" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K44" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="45">
       <c r="C45" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>